<commit_message>
Inclusão da validação do CPF e alterações nas documentações
</commit_message>
<xml_diff>
--- a/Arquivos/Visão e Backlog.xlsx
+++ b/Arquivos/Visão e Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa075dabe18a2777/Documentos/FATEC - ADS/2º SEM (24.02)/Engenharia de Software I/PROJETO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa075dabe18a2777/Documentos/PROGRAMAS/1.GIT/projeto-ESI/Arquivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{0C0DC296-6F17-450A-9F59-E45A4964A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E6931FE-F8D9-4E1F-9F67-CD8392494677}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="8_{0C0DC296-6F17-450A-9F59-E45A4964A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6604616B-FB6B-4AEC-95AD-47ED72EEED81}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$E$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$F$18</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$B$1:$F$20</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>Nome do Aplicativo</t>
   </si>
@@ -140,16 +140,81 @@
     <t>Verificar Disponibilidade de Salas</t>
   </si>
   <si>
-    <t>COMO administrador do sistema, quero cadastrar novas salas com informações como nome, número de sala, capacidade e equipamentos, para que possam ser reservadas pelos usuários.</t>
-  </si>
-  <si>
-    <t>COMO administrador do sistema, quero cadastrar novos usuários, fornecendo-lhes permissões e identificações específicas, para que possam acessar o sistema de reservas de acordo com suas permissões.</t>
-  </si>
-  <si>
-    <t>COMO usuário do sistema, quero visualizar a lista de salas cadastradas, com informações sobre sua capacidade e equipamentos, para escolher a sala que melhor atende à necessidade da reunião.</t>
-  </si>
-  <si>
-    <t>ReuniOn</t>
+    <t>Alterar Reserva</t>
+  </si>
+  <si>
+    <t>Detalhamento</t>
+  </si>
+  <si>
+    <t>Reservar Sala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Como USUÁRIO, quero reservar uma sala específica, garantindo que ela esteja disponível para minha reunião. </t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, quero alterar uma reserva já efetuada.</t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, quero cancelar uma reserva efetuada.</t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, quero verificar a disponibilidade de uma sala para saber se o horário desejado está ocupado antes de fazer a reserva.</t>
+  </si>
+  <si>
+    <t>O usuário deverá apontar qual reserva deseja cancelar dentre todas as suas próprias reservas.
+O sistema deverá exibir uma lista com todas as reservas feitas utilizando o id do usuário em questão</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O usuário deverá apontar:
+- O tipo de sala que deseja verificar;
+- A data que deseja verificar;
+O sistema deverá exibir uma lista com todas as salas do tipo escolhido, mostrando todos horários </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>indisponíveis</t>
+    </r>
+  </si>
+  <si>
+    <t>ReuniON</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero cadastrar novas salas no sistema</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero cadastrar novos usuários no sistema</t>
+  </si>
+  <si>
+    <t>Como ADMINSITRADOR, quero alterar uma sala  já cadastrada.</t>
+  </si>
+  <si>
+    <t>Para efetuar a reserva, o usuário deve apontar:
+- A sala escolhida, dentre as exibidas pelo sistema;
+- Data e hora do início da reserva;
+- Data e hora do fim da reserva;
+O sistema deverá fazer a validação da disponibilidade com os parâmetros inseridos.</t>
+  </si>
+  <si>
+    <t>O administrador deverá apontar:
+- Qual sala deseja modificar dentre todas as exibidas pelo sistema;
+- Os dados a serem alterados (número, tipo de sala e status)
+O sistema deverá:
+- Exibir uma lista com todas as salas cadastradas.
+- Em caso de mudança de status, deverá verificar se não há nenhum agendamento programado.</t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, desejo ver todas as reservas efetuadas utilizando meu id e senha.</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero alterar um usuário cadastrado</t>
   </si>
   <si>
     <r>
@@ -158,43 +223,113 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>ReuniOn</t>
+      <t>ReuniON</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> é um sistema de controle de reservas que oferece, de forma prática e eficiente, a possibilidade de reservar e gerenciar salas conforme a necessidade, permitindo controle de horários e permissões de acesso. Diferentemente de outras soluções convencionais, o </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>ReuniOn</t>
+      <t>ReuniON</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="12"/>
         <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> tem uma interface de linha de comando simples e eficaz, permitindo consultas em tempo real, proporcionando maior organização e eficiência no uso dos espaços corporativos.</t>
     </r>
+  </si>
+  <si>
+    <t>O usuário deverá apontar:
+- Qual reserva deseja modificar dentre todas as suas próprias reservas;
+- Os dados a serem alterados (início e fim da reserva, tipo de sala)
+O sistema deverá:
+- Exibir uma lista com todas as reservas feitas utilizando o id do usuário em questão;
+- Fazer a validação da disponibilidade com os novos parâmetros inseridos.</t>
+  </si>
+  <si>
+    <t>o administrador deverá apontar:
+- O número da sala
+- O tipo da sala (PA, PC, MA, MC ou GA)**
+- O status da sala (Ativa,  Em manutenção, Inativa)
+O sistema deverá validar se o número de sala já não foi utilizado</t>
+  </si>
+  <si>
+    <t>* O perfil ADMINISTRADOR pode executar todas as funções atribuídas ao perfil USUÁRIO.
+** Legenda:
+PA - Sala P (até 5 lugares), com recursos audiovisuais
+MA - Sala M (até 15 lugares), com recursos audiovisuais
+GA - Auditório (até 100 lugares), com recursos audiovisuais
+PC - Sala P (até 5 lugares), sem recursos audiovisuais
+MC - Sala M (até 15 lugares), sem recursos audiovisuais</t>
+  </si>
+  <si>
+    <t>Listar usuários</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero listar todos os usuários cadastrados no sistema</t>
+  </si>
+  <si>
+    <t>O sistema deverá exibir uma lista de todos os usários cadastros, com os dados completos para cada um.</t>
+  </si>
+  <si>
+    <t>O administrador deverá apontar:
+- Qual usuário deseja modificar dentre todas os exibidos pelo sistema;
+- Os dados a serem alterados (CPF, nome, perfil, senha e status)
+O sistema deverá:
+- Exibir uma lista com todas as salas cadastradas.
+- Em caso de mudança de status, deverá verificar se não há nenhum agendamento programado.</t>
+  </si>
+  <si>
+    <t>o administrador deverá apontar:
+- CPF
+- Nome do usuário
+- Perfil (usuário geral ou administrador)
+- Senha
+- O status do usuário (Ativo,  Inativo)
+O sistema deverá:
+- Validar o CPF
+- Validar se o documento já não foi utilizado para outro usuário
+- Gerar um id sequencial e automático, com uma sequência de 5 dígitos, sendo o id 00001 reservado para o perfil "Master"</t>
+  </si>
+  <si>
+    <t>Alterar senha</t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, desejo alterar minha senha de acesso.</t>
+  </si>
+  <si>
+    <t>O usuário deverá apontar a senha atual e a nova senha.
+O sistema deverá validar a senha atual.</t>
+  </si>
+  <si>
+    <t>O sistema exibirá uma lista com todas as reservas efetuadas pelo usuário em questão, exibindo o status da reserva.</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero listar todas as reservas efetuadas no período estipulado para o tipo de sala específico</t>
+  </si>
+  <si>
+    <t>O administrador deverá apontar o tipo de sala e o período que deseja consultar.</t>
   </si>
 </sst>
 </file>
@@ -218,32 +353,31 @@
       <charset val="1"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
+      <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -267,7 +401,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -384,51 +518,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top style="medium">
         <color auto="1"/>
@@ -462,70 +551,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -936,281 +1060,318 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:E20"/>
+  <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScale="71" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="35" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.44140625" style="11"/>
-    <col min="3" max="3" width="10.109375" style="11" customWidth="1"/>
-    <col min="4" max="4" width="36.5546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="64.44140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" style="4"/>
+    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="46.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.44140625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-    </row>
-    <row r="2" spans="2:5" s="2" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="17" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="2:6" ht="88.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="22"/>
+    </row>
+    <row r="5" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="2:6" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="105" x14ac:dyDescent="0.3">
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10">
+        <v>100</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-    </row>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-    </row>
-    <row r="4" spans="2:5" ht="88.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="19" t="s">
+      <c r="F7" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="165" x14ac:dyDescent="0.3">
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+      <c r="C8" s="10">
+        <v>95</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-    </row>
-    <row r="6" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="F8" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="75" x14ac:dyDescent="0.3">
+      <c r="B9" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C9" s="10">
+        <v>90</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="90.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="C10" s="10">
+        <v>85</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="105" x14ac:dyDescent="0.3">
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="C11" s="10">
+        <v>80</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="180" x14ac:dyDescent="0.3">
+      <c r="B12" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B7" s="12">
-        <v>1</v>
-      </c>
-      <c r="C7" s="7">
-        <v>100</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C12" s="10">
+        <v>75</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="135" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
         <v>7</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="12">
-        <v>2</v>
-      </c>
-      <c r="C8" s="7">
-        <v>95</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" s="12">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7">
-        <v>90</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="12">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7">
-        <v>85</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" s="12">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7">
-        <v>80</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C13" s="10">
+        <v>70</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="B14" s="9">
+        <v>8</v>
+      </c>
+      <c r="C14" s="10">
+        <v>65</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="150" x14ac:dyDescent="0.3">
+      <c r="B15" s="9">
         <v>9</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B12" s="12">
-        <v>6</v>
-      </c>
-      <c r="C12" s="7">
-        <v>75</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="C15" s="10">
+        <v>60</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="45" x14ac:dyDescent="0.3">
+      <c r="B16" s="9">
+        <v>10</v>
+      </c>
+      <c r="C16" s="10">
+        <v>55</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="B17" s="9">
+        <v>11</v>
+      </c>
+      <c r="C17" s="10">
+        <v>50</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.3">
+      <c r="B18" s="9">
+        <v>12</v>
+      </c>
+      <c r="C18" s="10">
+        <v>45</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B13" s="12">
-        <v>7</v>
-      </c>
-      <c r="C13" s="7">
-        <v>70</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="12">
-        <v>8</v>
-      </c>
-      <c r="C14" s="7">
-        <v>65</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="12">
-        <v>9</v>
-      </c>
-      <c r="C15" s="7">
-        <v>60</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B16" s="12">
-        <v>10</v>
-      </c>
-      <c r="C16" s="7">
-        <v>55</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="12">
-        <v>11</v>
-      </c>
-      <c r="C17" s="7">
-        <v>50</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B18" s="12">
-        <v>12</v>
-      </c>
-      <c r="C18" s="7">
-        <v>45</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B19" s="12">
-        <v>13</v>
-      </c>
-      <c r="C19" s="7">
-        <v>40</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="13">
-        <v>14</v>
-      </c>
-      <c r="C20" s="14">
-        <v>35</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>30</v>
-      </c>
+      <c r="E18" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="2:6" ht="115.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B4:E4"/>
+  <autoFilter ref="B1:F18" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0" showButton="0"/>
+    <filterColumn colId="1" showButton="0"/>
+    <filterColumn colId="2" showButton="0"/>
+    <filterColumn colId="3" showButton="0"/>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:F18">
+    <sortCondition descending="1" ref="C7:C18"/>
+  </sortState>
+  <mergeCells count="6">
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1225,198 +1386,198 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="11">
+      <c r="A1" s="4">
         <v>1</v>
       </c>
-      <c r="B1" s="11">
+      <c r="B1" s="4">
         <v>100</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="4">
         <v>90</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="4">
         <v>3</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="4">
         <v>80</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="4">
         <v>4</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="4">
         <v>85</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="4">
         <v>5</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="4">
         <v>95</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="4">
         <v>6</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="4">
         <v>75</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="4">
         <v>7</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="4">
         <v>80</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="4">
         <v>8</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="4">
         <v>100</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="4">
         <v>9</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="4">
         <v>90</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="11">
+      <c r="A10" s="4">
         <v>10</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="4">
         <v>85</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
+      <c r="A11" s="4">
         <v>11</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="4">
         <v>70</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="11">
+      <c r="A12" s="4">
         <v>12</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="4">
         <v>65</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="11">
+      <c r="A13" s="4">
         <v>13</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="4">
         <v>95</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="4" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="11">
+      <c r="A14" s="4">
         <v>14</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="4">
         <v>80</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DOCS: Descrição de casos de uso e requisitos não-funcionais
</commit_message>
<xml_diff>
--- a/Arquivos/Visão e Backlog.xlsx
+++ b/Arquivos/Visão e Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa075dabe18a2777/Documentos/PROGRAMAS/1.GIT/projeto-ESI/Arquivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="256" documentId="8_{0C0DC296-6F17-450A-9F59-E45A4964A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6604616B-FB6B-4AEC-95AD-47ED72EEED81}"/>
+  <xr:revisionPtr revIDLastSave="258" documentId="8_{0C0DC296-6F17-450A-9F59-E45A4964A868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBA943AA-E2DE-4B01-A594-E00B0742FD6B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$1:$F$18</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Planilha1!$B$1:$F$20</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -165,6 +165,154 @@
 O sistema deverá exibir uma lista com todas as reservas feitas utilizando o id do usuário em questão</t>
   </si>
   <si>
+    <t>ReuniON</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero cadastrar novas salas no sistema</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero cadastrar novos usuários no sistema</t>
+  </si>
+  <si>
+    <t>Como ADMINSITRADOR, quero alterar uma sala  já cadastrada.</t>
+  </si>
+  <si>
+    <t>Para efetuar a reserva, o usuário deve apontar:
+- A sala escolhida, dentre as exibidas pelo sistema;
+- Data e hora do início da reserva;
+- Data e hora do fim da reserva;
+O sistema deverá fazer a validação da disponibilidade com os parâmetros inseridos.</t>
+  </si>
+  <si>
+    <t>O administrador deverá apontar:
+- Qual sala deseja modificar dentre todas as exibidas pelo sistema;
+- Os dados a serem alterados (número, tipo de sala e status)
+O sistema deverá:
+- Exibir uma lista com todas as salas cadastradas.
+- Em caso de mudança de status, deverá verificar se não há nenhum agendamento programado.</t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, desejo ver todas as reservas efetuadas utilizando meu id e senha.</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero alterar um usuário cadastrado</t>
+  </si>
+  <si>
+    <t>O usuário deverá apontar:
+- Qual reserva deseja modificar dentre todas as suas próprias reservas;
+- Os dados a serem alterados (início e fim da reserva, tipo de sala)
+O sistema deverá:
+- Exibir uma lista com todas as reservas feitas utilizando o id do usuário em questão;
+- Fazer a validação da disponibilidade com os novos parâmetros inseridos.</t>
+  </si>
+  <si>
+    <t>o administrador deverá apontar:
+- O número da sala
+- O tipo da sala (PA, PC, MA, MC ou GA)**
+- O status da sala (Ativa,  Em manutenção, Inativa)
+O sistema deverá validar se o número de sala já não foi utilizado</t>
+  </si>
+  <si>
+    <t>* O perfil ADMINISTRADOR pode executar todas as funções atribuídas ao perfil USUÁRIO.
+** Legenda:
+PA - Sala P (até 5 lugares), com recursos audiovisuais
+MA - Sala M (até 15 lugares), com recursos audiovisuais
+GA - Auditório (até 100 lugares), com recursos audiovisuais
+PC - Sala P (até 5 lugares), sem recursos audiovisuais
+MC - Sala M (até 15 lugares), sem recursos audiovisuais</t>
+  </si>
+  <si>
+    <t>Listar usuários</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero listar todos os usuários cadastrados no sistema</t>
+  </si>
+  <si>
+    <t>O sistema deverá exibir uma lista de todos os usários cadastros, com os dados completos para cada um.</t>
+  </si>
+  <si>
+    <t>O administrador deverá apontar:
+- Qual usuário deseja modificar dentre todas os exibidos pelo sistema;
+- Os dados a serem alterados (CPF, nome, perfil, senha e status)
+O sistema deverá:
+- Exibir uma lista com todas as salas cadastradas.
+- Em caso de mudança de status, deverá verificar se não há nenhum agendamento programado.</t>
+  </si>
+  <si>
+    <t>o administrador deverá apontar:
+- CPF
+- Nome do usuário
+- Perfil (usuário geral ou administrador)
+- Senha
+- O status do usuário (Ativo,  Inativo)
+O sistema deverá:
+- Validar o CPF
+- Validar se o documento já não foi utilizado para outro usuário
+- Gerar um id sequencial e automático, com uma sequência de 5 dígitos, sendo o id 00001 reservado para o perfil "Master"</t>
+  </si>
+  <si>
+    <t>Alterar senha</t>
+  </si>
+  <si>
+    <t>Como USUÁRIO, desejo alterar minha senha de acesso.</t>
+  </si>
+  <si>
+    <t>O usuário deverá apontar a senha atual e a nova senha.
+O sistema deverá validar a senha atual.</t>
+  </si>
+  <si>
+    <t>O sistema exibirá uma lista com todas as reservas efetuadas pelo usuário em questão, exibindo o status da reserva.</t>
+  </si>
+  <si>
+    <t>Como ADMINISTRADOR, quero listar todas as reservas efetuadas no período estipulado para o tipo de sala específico</t>
+  </si>
+  <si>
+    <t>O administrador deverá apontar o tipo de sala e o período que deseja consultar.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Para empresas que desejam otimizar o uso de suas salas de reunião e evitar conflitos de agendamento, o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ReuniON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> é um sistema de controle de reservas que oferece, de forma prática e eficiente, a possibilidade de reservar e gerenciar salas conforme a necessidade, permitindo controle de horários e permissões de acesso. Diferentemente de outras soluções convencionais, o </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ReuniON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> tem uma interface de linha de comando simples e eficaz, permitindo consultas em tempo real, proporcionando maior organização e eficiência no uso dos espaços corporativos.</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">O usuário deverá apontar:
 - O tipo de sala que deseja verificar;
@@ -175,7 +323,7 @@
       <rPr>
         <b/>
         <i/>
-        <sz val="12"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -183,160 +331,12 @@
       <t>indisponíveis</t>
     </r>
   </si>
-  <si>
-    <t>ReuniON</t>
-  </si>
-  <si>
-    <t>Como ADMINISTRADOR, quero cadastrar novas salas no sistema</t>
-  </si>
-  <si>
-    <t>Como ADMINISTRADOR, quero cadastrar novos usuários no sistema</t>
-  </si>
-  <si>
-    <t>Como ADMINSITRADOR, quero alterar uma sala  já cadastrada.</t>
-  </si>
-  <si>
-    <t>Para efetuar a reserva, o usuário deve apontar:
-- A sala escolhida, dentre as exibidas pelo sistema;
-- Data e hora do início da reserva;
-- Data e hora do fim da reserva;
-O sistema deverá fazer a validação da disponibilidade com os parâmetros inseridos.</t>
-  </si>
-  <si>
-    <t>O administrador deverá apontar:
-- Qual sala deseja modificar dentre todas as exibidas pelo sistema;
-- Os dados a serem alterados (número, tipo de sala e status)
-O sistema deverá:
-- Exibir uma lista com todas as salas cadastradas.
-- Em caso de mudança de status, deverá verificar se não há nenhum agendamento programado.</t>
-  </si>
-  <si>
-    <t>Como USUÁRIO, desejo ver todas as reservas efetuadas utilizando meu id e senha.</t>
-  </si>
-  <si>
-    <t>Como ADMINISTRADOR, quero alterar um usuário cadastrado</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Para empresas que desejam otimizar o uso de suas salas de reunião e evitar conflitos de agendamento, o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ReuniON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> é um sistema de controle de reservas que oferece, de forma prática e eficiente, a possibilidade de reservar e gerenciar salas conforme a necessidade, permitindo controle de horários e permissões de acesso. Diferentemente de outras soluções convencionais, o </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ReuniON</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> tem uma interface de linha de comando simples e eficaz, permitindo consultas em tempo real, proporcionando maior organização e eficiência no uso dos espaços corporativos.</t>
-    </r>
-  </si>
-  <si>
-    <t>O usuário deverá apontar:
-- Qual reserva deseja modificar dentre todas as suas próprias reservas;
-- Os dados a serem alterados (início e fim da reserva, tipo de sala)
-O sistema deverá:
-- Exibir uma lista com todas as reservas feitas utilizando o id do usuário em questão;
-- Fazer a validação da disponibilidade com os novos parâmetros inseridos.</t>
-  </si>
-  <si>
-    <t>o administrador deverá apontar:
-- O número da sala
-- O tipo da sala (PA, PC, MA, MC ou GA)**
-- O status da sala (Ativa,  Em manutenção, Inativa)
-O sistema deverá validar se o número de sala já não foi utilizado</t>
-  </si>
-  <si>
-    <t>* O perfil ADMINISTRADOR pode executar todas as funções atribuídas ao perfil USUÁRIO.
-** Legenda:
-PA - Sala P (até 5 lugares), com recursos audiovisuais
-MA - Sala M (até 15 lugares), com recursos audiovisuais
-GA - Auditório (até 100 lugares), com recursos audiovisuais
-PC - Sala P (até 5 lugares), sem recursos audiovisuais
-MC - Sala M (até 15 lugares), sem recursos audiovisuais</t>
-  </si>
-  <si>
-    <t>Listar usuários</t>
-  </si>
-  <si>
-    <t>Como ADMINISTRADOR, quero listar todos os usuários cadastrados no sistema</t>
-  </si>
-  <si>
-    <t>O sistema deverá exibir uma lista de todos os usários cadastros, com os dados completos para cada um.</t>
-  </si>
-  <si>
-    <t>O administrador deverá apontar:
-- Qual usuário deseja modificar dentre todas os exibidos pelo sistema;
-- Os dados a serem alterados (CPF, nome, perfil, senha e status)
-O sistema deverá:
-- Exibir uma lista com todas as salas cadastradas.
-- Em caso de mudança de status, deverá verificar se não há nenhum agendamento programado.</t>
-  </si>
-  <si>
-    <t>o administrador deverá apontar:
-- CPF
-- Nome do usuário
-- Perfil (usuário geral ou administrador)
-- Senha
-- O status do usuário (Ativo,  Inativo)
-O sistema deverá:
-- Validar o CPF
-- Validar se o documento já não foi utilizado para outro usuário
-- Gerar um id sequencial e automático, com uma sequência de 5 dígitos, sendo o id 00001 reservado para o perfil "Master"</t>
-  </si>
-  <si>
-    <t>Alterar senha</t>
-  </si>
-  <si>
-    <t>Como USUÁRIO, desejo alterar minha senha de acesso.</t>
-  </si>
-  <si>
-    <t>O usuário deverá apontar a senha atual e a nova senha.
-O sistema deverá validar a senha atual.</t>
-  </si>
-  <si>
-    <t>O sistema exibirá uma lista com todas as reservas efetuadas pelo usuário em questão, exibindo o status da reserva.</t>
-  </si>
-  <si>
-    <t>Como ADMINISTRADOR, quero listar todas as reservas efetuadas no período estipulado para o tipo de sala específico</t>
-  </si>
-  <si>
-    <t>O administrador deverá apontar o tipo de sala e o período que deseja consultar.</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -354,20 +354,20 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <i/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -375,10 +375,17 @@
     <font>
       <b/>
       <i/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -581,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -594,12 +601,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -618,37 +649,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1062,8 +1078,8 @@
   </sheetPr>
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="35" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="35" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,284 +1088,290 @@
     <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="36.5546875" style="4" customWidth="1"/>
     <col min="5" max="5" width="46.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.44140625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="64.44140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-    </row>
-    <row r="2" spans="2:6" s="2" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="2:6" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="17" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+    </row>
+    <row r="2" spans="2:6" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="2:6" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="2:6" ht="88.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22"/>
-    </row>
-    <row r="5" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="17" t="s">
+      <c r="B4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-    </row>
-    <row r="6" spans="2:6" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="105" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
+    <row r="7" spans="2:6" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="B7" s="17">
         <v>1</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="18">
         <v>100</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="17">
+        <v>2</v>
+      </c>
+      <c r="C8" s="18">
+        <v>95</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="66" x14ac:dyDescent="0.3">
+      <c r="B9" s="17">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18">
+        <v>90</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="17">
+        <v>4</v>
+      </c>
+      <c r="C10" s="18">
+        <v>85</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="B11" s="17">
+        <v>5</v>
+      </c>
+      <c r="C11" s="18">
+        <v>80</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="B12" s="17">
+        <v>6</v>
+      </c>
+      <c r="C12" s="18">
+        <v>75</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="17">
+        <v>7</v>
+      </c>
+      <c r="C13" s="18">
+        <v>70</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="165" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
-        <v>2</v>
-      </c>
-      <c r="C8" s="10">
-        <v>95</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="13" t="s">
+    <row r="14" spans="2:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B14" s="17">
+        <v>8</v>
+      </c>
+      <c r="C14" s="18">
+        <v>65</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="17">
+        <v>9</v>
+      </c>
+      <c r="C15" s="18">
+        <v>60</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="17">
+        <v>10</v>
+      </c>
+      <c r="C16" s="18">
+        <v>55</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B17" s="17">
+        <v>11</v>
+      </c>
+      <c r="C17" s="18">
+        <v>50</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="17">
+        <v>12</v>
+      </c>
+      <c r="C18" s="18">
+        <v>45</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" spans="2:6" ht="115.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="25" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="75" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
-        <v>3</v>
-      </c>
-      <c r="C9" s="10">
-        <v>90</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" ht="90.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
-        <v>4</v>
-      </c>
-      <c r="C10" s="10">
-        <v>85</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="105" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
-        <v>5</v>
-      </c>
-      <c r="C11" s="10">
-        <v>80</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="180" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
-        <v>6</v>
-      </c>
-      <c r="C12" s="10">
-        <v>75</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" ht="135" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
-        <v>7</v>
-      </c>
-      <c r="C13" s="10">
-        <v>70</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="B14" s="9">
-        <v>8</v>
-      </c>
-      <c r="C14" s="10">
-        <v>65</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="150" x14ac:dyDescent="0.3">
-      <c r="B15" s="9">
-        <v>9</v>
-      </c>
-      <c r="C15" s="10">
-        <v>60</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" ht="45" x14ac:dyDescent="0.3">
-      <c r="B16" s="9">
-        <v>10</v>
-      </c>
-      <c r="C16" s="10">
-        <v>55</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
-        <v>11</v>
-      </c>
-      <c r="C17" s="10">
-        <v>50</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" ht="45" x14ac:dyDescent="0.3">
-      <c r="B18" s="9">
-        <v>12</v>
-      </c>
-      <c r="C18" s="10">
-        <v>45</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="2:6" ht="115.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="27"/>
     </row>
   </sheetData>
   <autoFilter ref="B1:F18" xr:uid="{00000000-0001-0000-0000-000000000000}">
@@ -1587,6 +1609,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101006DBEA977C939D641AD2F6529E45A8A07" ma:contentTypeVersion="12" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="956cb7e7140358a838be6477301e587e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5e6068a0-4fe6-4657-8f81-88092a9000c1" xmlns:ns3="a4dace15-48bf-45d2-9fd8-484a8e8dd001" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="215a6def8c46eb79d56eee81b38b3884" ns2:_="" ns3:_="">
     <xsd:import namespace="5e6068a0-4fe6-4657-8f81-88092a9000c1"/>
@@ -1787,16 +1818,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CD3531-7D5B-48A2-A987-78819F3DBF34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4AEAA8A-0049-4881-B00B-9AFD91C3F510}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1813,12 +1843,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03CD3531-7D5B-48A2-A987-78819F3DBF34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>